<commit_message>
validate change after solving the enpoint file
</commit_message>
<xml_diff>
--- a/endpointAPI.xlsx
+++ b/endpointAPI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t xml:space="preserve">VERBE</t>
   </si>
@@ -137,9 +137,6 @@
     <t xml:space="preserve">retourne l’ensemble des posts</t>
   </si>
   <si>
-    <t xml:space="preserve">InProgress</t>
-  </si>
-  <si>
     <t xml:space="preserve">AD</t>
   </si>
   <si>
@@ -407,6 +404,9 @@
     <t xml:space="preserve">retourne l’ensemble des posts du user dont l’id est userid</t>
   </si>
   <si>
+    <t xml:space="preserve">OD</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="22"/>
@@ -444,11 +444,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">users/userid/comments’</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">retourne l’ensemble des commentaires du user dont l’id est userid</t>
+      <t xml:space="preserve">users/userid/todos’</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">retourne l’ensemble des todos du user dont l’id est userid</t>
   </si>
   <si>
     <r>
@@ -488,11 +488,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">users/userid/todos’</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">retourne l’ensemble des todos du user dont l’id est userid</t>
+      <t xml:space="preserve">users/userid/albums’</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">retourne l’ensemble des albums du user dont l’id est userid</t>
   </si>
   <si>
     <r>
@@ -532,51 +532,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">users/userid/albums’</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">retourne l’ensemble des albums du user dont l’id est userid</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color rgb="FFEEEEEE"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">'</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="22"/>
-        <color rgb="FFFF8000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">groupe4/api</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color rgb="FFFF8000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color rgb="FFEEEEEE"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">users/userid/albums/photos’</t>
+      <t xml:space="preserve">users/userid/photos’</t>
     </r>
   </si>
   <si>
@@ -675,8 +631,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$mk-40B];[RED]\-#,##0.00\ [$mk-40B]"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -783,7 +740,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,8 +785,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFE8A202"/>
+        <fgColor rgb="FFFF4000"/>
+        <bgColor rgb="FFFF8000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA1467E"/>
+        <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
   </fills>
@@ -867,7 +830,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -924,7 +887,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -936,11 +899,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -957,7 +928,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFEEEEEE"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF38"/>
@@ -972,7 +943,7 @@
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFA1467E"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
@@ -1021,10 +992,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="22.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1081,11 +1052,11 @@
       <c r="C3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,15 +1064,15 @@
         <v>5</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1110,15 +1081,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1127,15 +1098,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1144,15 +1115,15 @@
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1161,15 +1132,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="14" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1178,13 +1149,17 @@
         <v>5</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="18"/>
     </row>
     <row r="10" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
@@ -1196,8 +1171,13 @@
       <c r="C10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
@@ -1209,8 +1189,12 @@
       <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
@@ -1222,8 +1206,13 @@
       <c r="C12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
@@ -1235,8 +1224,12 @@
       <c r="C13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
@@ -1248,28 +1241,26 @@
       <c r="C14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="18"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="18"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
begin to implemet POST method
</commit_message>
<xml_diff>
--- a/endpointAPI.xlsx
+++ b/endpointAPI.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t xml:space="preserve">VERBE</t>
   </si>
@@ -110,6 +110,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -119,6 +120,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -137,9 +139,6 @@
     <t xml:space="preserve">retourne l’ensemble des posts</t>
   </si>
   <si>
-    <t xml:space="preserve">InProgress</t>
-  </si>
-  <si>
     <t xml:space="preserve">AD</t>
   </si>
   <si>
@@ -160,6 +159,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -169,6 +169,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -204,6 +205,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -213,6 +215,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -248,6 +251,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -257,6 +261,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -292,6 +297,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -301,6 +307,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -336,6 +343,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -345,6 +353,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -380,6 +389,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -389,6 +399,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -407,6 +418,9 @@
     <t xml:space="preserve">retourne l’ensemble des posts du user dont l’id est userid</t>
   </si>
   <si>
+    <t xml:space="preserve">OD</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="22"/>
@@ -424,6 +438,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -433,6 +448,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -468,6 +484,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -477,6 +494,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -512,6 +530,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -521,6 +540,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -556,6 +576,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -565,6 +586,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -576,7 +598,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">users/userid/albums/photos’</t>
+      <t xml:space="preserve">users/userid/photos’</t>
     </r>
   </si>
   <si>
@@ -600,6 +622,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -609,6 +632,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -644,6 +668,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">groupe4/api</t>
     </r>
@@ -653,6 +678,7 @@
         <color rgb="FFFF8000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">/</t>
     </r>
@@ -678,7 +704,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -763,19 +789,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="22"/>
-      <color rgb="FFFF8000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FFFF8000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color rgb="FFEEEEEE"/>
       <name val="Arial"/>
@@ -783,7 +796,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -826,12 +839,6 @@
         <bgColor rgb="FF168253"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFE8A202"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -867,7 +874,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -934,10 +941,6 @@
     </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1032,7 +1035,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="65.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="114.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="24.6"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="5" width="11.52"/>
   </cols>
@@ -1081,11 +1084,11 @@
       <c r="C3" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,15 +1096,15 @@
         <v>5</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1110,15 +1113,15 @@
         <v>5</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1127,15 +1130,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1144,15 +1147,15 @@
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1161,15 +1164,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1178,13 +1181,17 @@
         <v>5</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="D9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="18"/>
     </row>
     <row r="10" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
@@ -1196,8 +1203,12 @@
       <c r="C10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
@@ -1209,8 +1220,12 @@
       <c r="C11" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
@@ -1222,8 +1237,12 @@
       <c r="C12" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
@@ -1235,8 +1254,12 @@
       <c r="C13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
@@ -1248,8 +1271,12 @@
       <c r="C14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
@@ -1261,15 +1288,19 @@
       <c r="C15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" s="15" customFormat="true" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>